<commit_message>
feat: 新增 ArgumentException 异常。Issues #9
</commit_message>
<xml_diff>
--- a/docs/MultipleLanguagesDeclaration.xlsx
+++ b/docs/MultipleLanguagesDeclaration.xlsx
@@ -1084,8 +1084,8 @@
   <sheetPr/>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="6"/>
@@ -1131,21 +1131,21 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="str">
-        <f>","""&amp;A2&amp;""": """&amp;B2&amp;""""</f>
+        <f t="shared" ref="C2:C9" si="0">","""&amp;A2&amp;""": """&amp;B2&amp;""""</f>
         <v>,"Exception": "应用程序引发了一个未处理的异常。"</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="2" t="str">
-        <f>","""&amp;A2&amp;""": """&amp;D2&amp;""""</f>
+        <f t="shared" ref="E2:E9" si="1">","""&amp;A2&amp;""": """&amp;D2&amp;""""</f>
         <v>,"Exception": "The application threw an unhandled exception."</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="2" t="str">
-        <f>","""&amp;A2&amp;""": """&amp;F2&amp;""""</f>
+        <f t="shared" ref="G2:G9" si="2">","""&amp;A2&amp;""": """&amp;F2&amp;""""</f>
         <v>,"Exception": "應用程序引發了一個未處理的異常。"</v>
       </c>
     </row>
@@ -1157,21 +1157,21 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="str">
-        <f>","""&amp;A3&amp;""": """&amp;B3&amp;""""</f>
+        <f t="shared" si="0"/>
         <v>,"ArgumentException": "错误的方法参数。"</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="2" t="str">
-        <f>","""&amp;A3&amp;""": """&amp;D3&amp;""""</f>
+        <f t="shared" si="1"/>
         <v>,"ArgumentException": "Bad method parameter value."</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="2" t="str">
-        <f>","""&amp;A3&amp;""": """&amp;F3&amp;""""</f>
+        <f t="shared" si="2"/>
         <v>,"ArgumentException": "錯誤的方法參數。"</v>
       </c>
     </row>
@@ -1183,21 +1183,21 @@
         <v>16</v>
       </c>
       <c r="C4" s="2" t="str">
-        <f>","""&amp;A4&amp;""": """&amp;B4&amp;""""</f>
+        <f t="shared" si="0"/>
         <v>,"ArgumentException_with_invalid_argument_name": "错误的方法参数：{0}。"</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="2" t="str">
-        <f>","""&amp;A4&amp;""": """&amp;D4&amp;""""</f>
+        <f t="shared" si="1"/>
         <v>,"ArgumentException_with_invalid_argument_name": "Bad method parameter (see {0}) value."</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="2" t="str">
-        <f>","""&amp;A4&amp;""": """&amp;F4&amp;""""</f>
+        <f t="shared" si="2"/>
         <v>,"ArgumentException_with_invalid_argument_name": "錯誤的方法參數：{0}。"</v>
       </c>
     </row>
@@ -1209,21 +1209,21 @@
         <v>20</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f>","""&amp;A5&amp;""": """&amp;B5&amp;""""</f>
+        <f t="shared" si="0"/>
         <v>,"ArgumentNullException": "指定的方法参数是必需的。"</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="2" t="str">
-        <f>","""&amp;A5&amp;""": """&amp;D5&amp;""""</f>
+        <f t="shared" si="1"/>
         <v>,"ArgumentNullException": "The specified method parameter is required."</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="2" t="str">
-        <f>","""&amp;A5&amp;""": """&amp;F5&amp;""""</f>
+        <f t="shared" si="2"/>
         <v>,"ArgumentNullException": "指定的方法參數是必需的。"</v>
       </c>
     </row>
@@ -1235,21 +1235,21 @@
         <v>24</v>
       </c>
       <c r="C6" s="2" t="str">
-        <f>","""&amp;A6&amp;""": """&amp;B6&amp;""""</f>
+        <f t="shared" si="0"/>
         <v>,"ArgumentNullException_with_argument_name": "方法参数 {0} 是必需的。"</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="2" t="str">
-        <f>","""&amp;A6&amp;""": """&amp;D6&amp;""""</f>
+        <f t="shared" si="1"/>
         <v>,"ArgumentNullException_with_argument_name": "The parameter {0} is required"</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="2" t="str">
-        <f>","""&amp;A6&amp;""": """&amp;F6&amp;""""</f>
+        <f t="shared" si="2"/>
         <v>,"ArgumentNullException_with_argument_name": "方法參數 {0} 是必需的。"</v>
       </c>
     </row>
@@ -1261,21 +1261,21 @@
         <v>28</v>
       </c>
       <c r="C7" s="2" t="str">
-        <f>","""&amp;A7&amp;""": """&amp;B7&amp;""""</f>
+        <f t="shared" si="0"/>
         <v>,"CurrencyAbbr_rmb": "RMB"</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="2" t="str">
-        <f>","""&amp;A7&amp;""": """&amp;D7&amp;""""</f>
+        <f t="shared" si="1"/>
         <v>,"CurrencyAbbr_rmb": "CNY"</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G7" s="2" t="str">
-        <f>","""&amp;A7&amp;""": """&amp;F7&amp;""""</f>
+        <f t="shared" si="2"/>
         <v>,"CurrencyAbbr_rmb": "CNY"</v>
       </c>
     </row>
@@ -1287,21 +1287,21 @@
         <v>31</v>
       </c>
       <c r="C8" s="2" t="str">
-        <f>","""&amp;A8&amp;""": """&amp;B8&amp;""""</f>
+        <f t="shared" si="0"/>
         <v>,"CurrencyAbbr_dollar": "USD"</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="2" t="str">
-        <f>","""&amp;A8&amp;""": """&amp;D8&amp;""""</f>
+        <f t="shared" si="1"/>
         <v>,"CurrencyAbbr_dollar": "USD"</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G8" s="2" t="str">
-        <f>","""&amp;A8&amp;""": """&amp;F8&amp;""""</f>
+        <f t="shared" si="2"/>
         <v>,"CurrencyAbbr_dollar": "USD"</v>
       </c>
     </row>
@@ -1313,21 +1313,21 @@
         <v>33</v>
       </c>
       <c r="C9" s="2" t="str">
-        <f>","""&amp;A9&amp;""": """&amp;B9&amp;""""</f>
+        <f t="shared" si="0"/>
         <v>,"CurrencyAbbr_euro": "EUR"</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="2" t="str">
-        <f>","""&amp;A9&amp;""": """&amp;D9&amp;""""</f>
+        <f t="shared" si="1"/>
         <v>,"CurrencyAbbr_euro": "EUR"</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="2" t="str">
-        <f>","""&amp;A9&amp;""": """&amp;F9&amp;""""</f>
+        <f t="shared" si="2"/>
         <v>,"CurrencyAbbr_euro": "EUR"</v>
       </c>
     </row>

</xml_diff>